<commit_message>
Fixed svg on intro page, added button
</commit_message>
<xml_diff>
--- a/PracticeData.xlsx
+++ b/PracticeData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="6975" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="6975" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>activity</t>
   </si>
@@ -118,6 +119,177 @@
   <si>
     <t>asin</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>1960</t>
+  </si>
+  <si>
+    <t>1961</t>
+  </si>
+  <si>
+    <t>1962</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>1964</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>1967</t>
+  </si>
+  <si>
+    <t>1968</t>
+  </si>
+  <si>
+    <t>1969</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>1972</t>
+  </si>
+  <si>
+    <t>1973</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>HydroElectric</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
 </sst>
 </file>
 
@@ -829,23 +1001,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="51812224"/>
-        <c:axId val="51810688"/>
+        <c:axId val="56955648"/>
+        <c:axId val="56957184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51812224"/>
+        <c:axId val="56955648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51810688"/>
+        <c:crossAx val="56957184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51810688"/>
+        <c:axId val="56957184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,7 +1025,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51812224"/>
+        <c:crossAx val="56955648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -866,7 +1038,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2809,23 +2981,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48573440"/>
-        <c:axId val="48571904"/>
+        <c:axId val="57737600"/>
+        <c:axId val="57739136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48573440"/>
+        <c:axId val="57737600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48571904"/>
+        <c:crossAx val="57739136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48571904"/>
+        <c:axId val="57739136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,20 +3005,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48573440"/>
+        <c:crossAx val="57737600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8374,7 +8545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="A1:B36"/>
     </sheetView>
   </sheetViews>
@@ -11265,4 +11436,1059 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection sqref="A1:F52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3.3777141575979162</v>
+      </c>
+      <c r="D2">
+        <v>3.5044754497007746</v>
+      </c>
+      <c r="E2">
+        <v>92.08906058672369</v>
+      </c>
+      <c r="F2">
+        <v>1.0287498059776141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>4.0539485667201527</v>
+      </c>
+      <c r="D3">
+        <v>3.7269612732555619</v>
+      </c>
+      <c r="E3">
+        <v>90.910273645864962</v>
+      </c>
+      <c r="F3">
+        <v>1.3088165141593304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>7.0989206221507102</v>
+      </c>
+      <c r="D4">
+        <v>3.6814494502547599</v>
+      </c>
+      <c r="E4">
+        <v>87.968456690801816</v>
+      </c>
+      <c r="F4">
+        <v>1.2511732367927058</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>7.4712597507973363E-2</v>
+      </c>
+      <c r="C5">
+        <v>10.916876210062904</v>
+      </c>
+      <c r="D5">
+        <v>3.5460366172063917</v>
+      </c>
+      <c r="E5">
+        <v>84.178603276107239</v>
+      </c>
+      <c r="F5">
+        <v>1.2837712991154993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>0.10981818181818183</v>
+      </c>
+      <c r="C6">
+        <v>11.893090909090908</v>
+      </c>
+      <c r="D6">
+        <v>3.1709090909090909</v>
+      </c>
+      <c r="E6">
+        <v>83.157818181818172</v>
+      </c>
+      <c r="F6">
+        <v>1.6683636363636363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>8.6954749563527917E-2</v>
+      </c>
+      <c r="C7">
+        <v>13.424998131831552</v>
+      </c>
+      <c r="D7">
+        <v>4.0658138760758948</v>
+      </c>
+      <c r="E7">
+        <v>80.221191144202223</v>
+      </c>
+      <c r="F7">
+        <v>2.2010420983268006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>0.10664550290795005</v>
+      </c>
+      <c r="C8">
+        <v>12.35289740950633</v>
+      </c>
+      <c r="D8">
+        <v>4.0736101982862314</v>
+      </c>
+      <c r="E8">
+        <v>81.224191168264284</v>
+      </c>
+      <c r="F8">
+        <v>2.2426557210352054</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>9.0477401347107966E-2</v>
+      </c>
+      <c r="C9">
+        <v>13.559783090778993</v>
+      </c>
+      <c r="D9">
+        <v>3.9348799252526567</v>
+      </c>
+      <c r="E9">
+        <v>79.196702601373119</v>
+      </c>
+      <c r="F9">
+        <v>3.2181569812481152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>0.50857880478440798</v>
+      </c>
+      <c r="C10">
+        <v>15.10833614953768</v>
+      </c>
+      <c r="D10">
+        <v>4.2508988770269749</v>
+      </c>
+      <c r="E10">
+        <v>75.455809598732429</v>
+      </c>
+      <c r="F10">
+        <v>4.6763765699185056</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>0.27069346651383658</v>
+      </c>
+      <c r="C11">
+        <v>15.07849598821025</v>
+      </c>
+      <c r="D11">
+        <v>3.0410799083019486</v>
+      </c>
+      <c r="E11">
+        <v>77.082651056165048</v>
+      </c>
+      <c r="F11">
+        <v>4.5270795808089082</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>0.49495971591126042</v>
+      </c>
+      <c r="C12">
+        <v>17.926419489098478</v>
+      </c>
+      <c r="D12">
+        <v>3.0408759402802703</v>
+      </c>
+      <c r="E12">
+        <v>75.478731528504341</v>
+      </c>
+      <c r="F12">
+        <v>3.0590133262056591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>1.9235190436048737</v>
+      </c>
+      <c r="C13">
+        <v>18.801080091780754</v>
+      </c>
+      <c r="D13">
+        <v>3.1447079559849072</v>
+      </c>
+      <c r="E13">
+        <v>73.235722367727078</v>
+      </c>
+      <c r="F13">
+        <v>2.8949705409023903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14">
+        <v>2.9297882800342911</v>
+      </c>
+      <c r="C14">
+        <v>17.154152124716102</v>
+      </c>
+      <c r="D14">
+        <v>3.7358761939974077</v>
+      </c>
+      <c r="E14">
+        <v>73.798892441706926</v>
+      </c>
+      <c r="F14">
+        <v>2.3812909595452751</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>5.6479352490549131</v>
+      </c>
+      <c r="C15">
+        <v>12.924270866888083</v>
+      </c>
+      <c r="D15">
+        <v>5.9978302805454655</v>
+      </c>
+      <c r="E15">
+        <v>72.072452338372557</v>
+      </c>
+      <c r="F15">
+        <v>3.3575112651389767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <v>5.1834999911821242</v>
+      </c>
+      <c r="C16">
+        <v>12.271308396381144</v>
+      </c>
+      <c r="D16">
+        <v>4.6117489374459906</v>
+      </c>
+      <c r="E16">
+        <v>74.305415939191931</v>
+      </c>
+      <c r="F16">
+        <v>3.6280267357988114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17">
+        <v>4.5365959289735818</v>
+      </c>
+      <c r="C17">
+        <v>13.110653962754441</v>
+      </c>
+      <c r="D17">
+        <v>5.5965786054569078</v>
+      </c>
+      <c r="E17">
+        <v>73.072758770030319</v>
+      </c>
+      <c r="F17">
+        <v>3.6834127327847557</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18">
+        <v>5.8399839045000341</v>
+      </c>
+      <c r="C18">
+        <v>13.723760981825498</v>
+      </c>
+      <c r="D18">
+        <v>4.4624773657031724</v>
+      </c>
+      <c r="E18">
+        <v>71.319495674334391</v>
+      </c>
+      <c r="F18">
+        <v>4.4172087720474815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <v>8.1800848378702344</v>
+      </c>
+      <c r="C19">
+        <v>15.002515324849547</v>
+      </c>
+      <c r="D19">
+        <v>3.8444100786892985</v>
+      </c>
+      <c r="E19">
+        <v>68.363113537416226</v>
+      </c>
+      <c r="F19">
+        <v>4.2779154478209831</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <v>9.099260149253297</v>
+      </c>
+      <c r="C20">
+        <v>14.555550047097318</v>
+      </c>
+      <c r="D20">
+        <v>2.9281991910343037</v>
+      </c>
+      <c r="E20">
+        <v>68.605773577092336</v>
+      </c>
+      <c r="F20">
+        <v>4.4810983736115046</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>9.8217816267995879</v>
+      </c>
+      <c r="C21">
+        <v>14.674890702013311</v>
+      </c>
+      <c r="D21">
+        <v>3.0475341817270474</v>
+      </c>
+      <c r="E21">
+        <v>67.979449193840324</v>
+      </c>
+      <c r="F21">
+        <v>4.1018072456907353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>10.188652961063873</v>
+      </c>
+      <c r="C22">
+        <v>16.022374744828252</v>
+      </c>
+      <c r="D22">
+        <v>2.4625078359828332</v>
+      </c>
+      <c r="E22">
+        <v>67.281757831964384</v>
+      </c>
+      <c r="F22">
+        <v>3.6964407224642226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>10.261486451877273</v>
+      </c>
+      <c r="C23">
+        <v>16.255954515187216</v>
+      </c>
+      <c r="D23">
+        <v>2.2204579214260103</v>
+      </c>
+      <c r="E23">
+        <v>68.128617528043847</v>
+      </c>
+      <c r="F23">
+        <v>2.6473902576448292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>9.8972760998479394</v>
+      </c>
+      <c r="C24">
+        <v>17.861928131994663</v>
+      </c>
+      <c r="D24">
+        <v>2.3314891738458083</v>
+      </c>
+      <c r="E24">
+        <v>66.553676400352131</v>
+      </c>
+      <c r="F24">
+        <v>2.8034150081709259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25">
+        <v>11.91918201211289</v>
+      </c>
+      <c r="C25">
+        <v>18.08596719221244</v>
+      </c>
+      <c r="D25">
+        <v>2.1562906112841134</v>
+      </c>
+      <c r="E25">
+        <v>65.21148517764756</v>
+      </c>
+      <c r="F25">
+        <v>2.1158325772993649</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26">
+        <v>11.947095032150294</v>
+      </c>
+      <c r="C26">
+        <v>19.214663280016474</v>
+      </c>
+      <c r="D26">
+        <v>1.4004256195510401</v>
+      </c>
+      <c r="E26">
+        <v>65.472872474314087</v>
+      </c>
+      <c r="F26">
+        <v>1.4301732225807191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27">
+        <v>13.187988930291342</v>
+      </c>
+      <c r="C27">
+        <v>17.318428450022878</v>
+      </c>
+      <c r="D27">
+        <v>1.4835152862216994</v>
+      </c>
+      <c r="E27">
+        <v>66.166568608223827</v>
+      </c>
+      <c r="F27">
+        <v>1.4767601490488331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28">
+        <v>15.212389002732241</v>
+      </c>
+      <c r="C28">
+        <v>15.295210040983607</v>
+      </c>
+      <c r="D28">
+        <v>1.4698599726775956</v>
+      </c>
+      <c r="E28">
+        <v>66.306992827868854</v>
+      </c>
+      <c r="F28">
+        <v>1.3161714480874318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29">
+        <v>15.568967254408062</v>
+      </c>
+      <c r="C29">
+        <v>16.976322418136018</v>
+      </c>
+      <c r="D29">
+        <v>1.2411083123425692</v>
+      </c>
+      <c r="E29">
+        <v>63.719093198992439</v>
+      </c>
+      <c r="F29">
+        <v>2.0274055415617132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30">
+        <v>16.38205756761031</v>
+      </c>
+      <c r="C30">
+        <v>18.142693341768148</v>
+      </c>
+      <c r="D30">
+        <v>1.8646212241024831</v>
+      </c>
+      <c r="E30">
+        <v>60.777123201012174</v>
+      </c>
+      <c r="F30">
+        <v>2.3410564605408823</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31">
+        <v>15.991286798859598</v>
+      </c>
+      <c r="C31">
+        <v>18.370999775763206</v>
+      </c>
+      <c r="D31">
+        <v>2.9701364641060959</v>
+      </c>
+      <c r="E31">
+        <v>58.331598167665057</v>
+      </c>
+      <c r="F31">
+        <v>3.6386424063811389</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32">
+        <v>15.137094147593256</v>
+      </c>
+      <c r="C32">
+        <v>17.056640410255557</v>
+      </c>
+      <c r="D32">
+        <v>2.0027342072562293</v>
+      </c>
+      <c r="E32">
+        <v>61.558456645803986</v>
+      </c>
+      <c r="F32">
+        <v>3.4163069116527431</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33">
+        <v>16.703345979337648</v>
+      </c>
+      <c r="C33">
+        <v>17.402514647141079</v>
+      </c>
+      <c r="D33">
+        <v>1.6957052753308512</v>
+      </c>
+      <c r="E33">
+        <v>60.626872070817626</v>
+      </c>
+      <c r="F33">
+        <v>2.7799575582001372</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34">
+        <v>15.488228431283984</v>
+      </c>
+      <c r="C34">
+        <v>17.304177181858197</v>
+      </c>
+      <c r="D34">
+        <v>2.5221083303381455</v>
+      </c>
+      <c r="E34">
+        <v>60.809296550504634</v>
+      </c>
+      <c r="F34">
+        <v>2.9972380203698403</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35">
+        <v>17.653448395747549</v>
+      </c>
+      <c r="C35">
+        <v>15.482309341742512</v>
+      </c>
+      <c r="D35">
+        <v>2.8751195695683469</v>
+      </c>
+      <c r="E35">
+        <v>60.805424370956004</v>
+      </c>
+      <c r="F35">
+        <v>2.2566465645713256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36">
+        <v>19.406017567886149</v>
+      </c>
+      <c r="C36">
+        <v>15.593883453038027</v>
+      </c>
+      <c r="D36">
+        <v>2.7780727154279585</v>
+      </c>
+      <c r="E36">
+        <v>59.357571809319509</v>
+      </c>
+      <c r="F36">
+        <v>1.6945217780961104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37">
+        <v>17.471986857260202</v>
+      </c>
+      <c r="C37">
+        <v>15.607539218399836</v>
+      </c>
+      <c r="D37">
+        <v>3.7838947866536903</v>
+      </c>
+      <c r="E37">
+        <v>59.985714413264169</v>
+      </c>
+      <c r="F37">
+        <v>1.6421281952839706</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38">
+        <v>16.191709618469304</v>
+      </c>
+      <c r="C38">
+        <v>15.707356408909307</v>
+      </c>
+      <c r="D38">
+        <v>3.2056328096500617</v>
+      </c>
+      <c r="E38">
+        <v>62.075230962300743</v>
+      </c>
+      <c r="F38">
+        <v>1.2549548024275259</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39">
+        <v>14.387726638772664</v>
+      </c>
+      <c r="C39">
+        <v>17.330369595536961</v>
+      </c>
+      <c r="D39">
+        <v>3.6267433751743376</v>
+      </c>
+      <c r="E39">
+        <v>61.139818688981876</v>
+      </c>
+      <c r="F39">
+        <v>1.6361576011157601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40">
+        <v>12.732329266143088</v>
+      </c>
+      <c r="C40">
+        <v>19.034663998333478</v>
+      </c>
+      <c r="D40">
+        <v>4.6098185877656679</v>
+      </c>
+      <c r="E40">
+        <v>59.092066397340695</v>
+      </c>
+      <c r="F40">
+        <v>2.5606740152657621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41">
+        <v>12.693951929803349</v>
+      </c>
+      <c r="C41">
+        <v>18.640630802580556</v>
+      </c>
+      <c r="D41">
+        <v>4.7348193697156029</v>
+      </c>
+      <c r="E41">
+        <v>59.722944321135863</v>
+      </c>
+      <c r="F41">
+        <v>2.0970903971879884</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42">
+        <v>12.021050337188488</v>
+      </c>
+      <c r="C42">
+        <v>19.41690499937252</v>
+      </c>
+      <c r="D42">
+        <v>5.5271170879596303</v>
+      </c>
+      <c r="E42">
+        <v>59.199367234922292</v>
+      </c>
+      <c r="F42">
+        <v>1.829767699918758</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43">
+        <v>13.004001492081793</v>
+      </c>
+      <c r="C43">
+        <v>19.988978941300147</v>
+      </c>
+      <c r="D43">
+        <v>6.1007494319915905</v>
+      </c>
+      <c r="E43">
+        <v>56.515819458103024</v>
+      </c>
+      <c r="F43">
+        <v>2.8644579334667166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44">
+        <v>12.56341926748043</v>
+      </c>
+      <c r="C44">
+        <v>19.601668779256034</v>
+      </c>
+      <c r="D44">
+        <v>5.6283040398697182</v>
+      </c>
+      <c r="E44">
+        <v>58.313122340549405</v>
+      </c>
+      <c r="F44">
+        <v>2.3112060390113749</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>12.703420621431553</v>
+      </c>
+      <c r="C45">
+        <v>19.105000152660878</v>
+      </c>
+      <c r="D45">
+        <v>5.6060467277988675</v>
+      </c>
+      <c r="E45">
+        <v>57.238500395222061</v>
+      </c>
+      <c r="F45">
+        <v>3.6608078813723197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46">
+        <v>15.067890275311946</v>
+      </c>
+      <c r="C46">
+        <v>16.879797954539772</v>
+      </c>
+      <c r="D46">
+        <v>5.7276220482941991</v>
+      </c>
+      <c r="E46">
+        <v>56.818617522275851</v>
+      </c>
+      <c r="F46">
+        <v>3.8693706083868871</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47">
+        <v>14.702100368510926</v>
+      </c>
+      <c r="C47">
+        <v>17.568402943614796</v>
+      </c>
+      <c r="D47">
+        <v>5.4870909361008131</v>
+      </c>
+      <c r="E47">
+        <v>58.083998766838171</v>
+      </c>
+      <c r="F47">
+        <v>2.4490721735116199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48">
+        <v>15.906965264607312</v>
+      </c>
+      <c r="C48">
+        <v>17.560436205866306</v>
+      </c>
+      <c r="D48">
+        <v>5.5014483905328513</v>
+      </c>
+      <c r="E48">
+        <v>57.699202410953212</v>
+      </c>
+      <c r="F48">
+        <v>1.5019744875425425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49">
+        <v>14.562820974125806</v>
+      </c>
+      <c r="C49">
+        <v>18.025953634864038</v>
+      </c>
+      <c r="D49">
+        <v>6.3396527365648421</v>
+      </c>
+      <c r="E49">
+        <v>57.741307899954982</v>
+      </c>
+      <c r="F49">
+        <v>1.5335105943852796</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50">
+        <v>14.658314350797266</v>
+      </c>
+      <c r="C50">
+        <v>17.477454987986395</v>
+      </c>
+      <c r="D50">
+        <v>6.3831247854713391</v>
+      </c>
+      <c r="E50">
+        <v>58.397977969856775</v>
+      </c>
+      <c r="F50">
+        <v>1.3803164102724124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51">
+        <v>14.991801009081065</v>
+      </c>
+      <c r="C51">
+        <v>15.194578883577645</v>
+      </c>
+      <c r="D51">
+        <v>6.216808180089302</v>
+      </c>
+      <c r="E51">
+        <v>60.327495386513199</v>
+      </c>
+      <c r="F51">
+        <v>1.3760045629166853</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52">
+        <v>15.10620649981772</v>
+      </c>
+      <c r="C52">
+        <v>15.815922111888908</v>
+      </c>
+      <c r="D52">
+        <v>6.6590187730147532</v>
+      </c>
+      <c r="E52">
+        <v>58.780138665453705</v>
+      </c>
+      <c r="F52">
+        <v>1.4736130946209443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed add_data long title problem
</commit_message>
<xml_diff>
--- a/PracticeData.xlsx
+++ b/PracticeData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="6975" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14355" windowHeight="6975" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -295,6 +296,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\-yy;@"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -331,13 +335,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,7 +354,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:layout/>
@@ -1001,23 +1006,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="56955648"/>
-        <c:axId val="56957184"/>
+        <c:axId val="59959936"/>
+        <c:axId val="83825024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56955648"/>
+        <c:axId val="59959936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56957184"/>
+        <c:crossAx val="83825024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56957184"/>
+        <c:axId val="83825024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1030,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56955648"/>
+        <c:crossAx val="59959936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1038,7 +1043,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1046,7 +1051,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -2981,23 +2986,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57737600"/>
-        <c:axId val="57739136"/>
+        <c:axId val="83872000"/>
+        <c:axId val="85864448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57737600"/>
+        <c:axId val="83872000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57739136"/>
+        <c:crossAx val="85864448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57739136"/>
+        <c:axId val="85864448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3005,7 +3010,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57737600"/>
+        <c:crossAx val="83872000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3017,7 +3022,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8421,7 +8426,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11442,7 +11447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F52"/>
     </sheetView>
   </sheetViews>
@@ -12491,4 +12496,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="6">
+        <v>36951</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="6">
+        <v>36982</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="6">
+        <v>37012</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>